<commit_message>
Deploying to gh-pages from @ phenopackets/core-ig@b023441eead59a64d5bd4c5eaf367c5c621c55ad 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-PhenotypicFeature.xlsx
+++ b/StructureDefinition-PhenotypicFeature.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="410">
   <si>
     <t>Path</t>
   </si>
@@ -746,10 +746,6 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">boolean
-</t>
-  </si>
-  <si>
     <t>true: observed; false: excluded</t>
   </si>
   <si>
@@ -760,6 +756,9 @@
   </si>
   <si>
     <t>An observation exists to have a value, though it might not if it is in error, or if it represents a group of observations.</t>
+  </si>
+  <si>
+    <t>https://github.com/phenopackets/core-ig/ValueSet/phenotypicFeatureVS</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -1264,6 +1263,10 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean
+</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -1479,7 +1482,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.40625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="67.6015625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
@@ -4117,19 +4120,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>236</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>237</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4154,13 +4157,11 @@
         <v>45</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X23" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="X23" s="2"/>
       <c r="Y23" t="s" s="2">
-        <v>45</v>
+        <v>237</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -7056,19 +7057,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>233</v>
+        <v>398</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7135,7 +7136,7 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>240</v>
@@ -7152,7 +7153,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7178,13 +7179,13 @@
         <v>153</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N49" t="s" s="2">
         <v>247</v>
@@ -7236,7 +7237,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7271,7 +7272,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7355,7 +7356,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7390,7 +7391,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7416,10 +7417,10 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>314</v>
@@ -7474,7 +7475,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>

</xml_diff>